<commit_message>
Update SBNation and Posts
</commit_message>
<xml_diff>
--- a/RSS_Links.xlsx
+++ b/RSS_Links.xlsx
@@ -1,15 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spodionew/Documents/GitHub/streamlit-example/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3E5922-0678-B040-AEB0-B52DF95E8CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="34300" yWindow="8420" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,9 +40,6 @@
     <t>https://www.skysports.com/rss/12040</t>
   </si>
   <si>
-    <t>https://www.sbnation.com/rss</t>
-  </si>
-  <si>
     <t>https://www.sportskeeda.com/feed</t>
   </si>
   <si>
@@ -233,13 +245,16 @@
   </si>
   <si>
     <t>http://www.sportsonearth.com/gen/hb/rss/writers.xml</t>
+  </si>
+  <si>
+    <t>https://rss.app/feeds/4vxPD1ijVbt2vi9d.xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +330,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -361,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,9 +416,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,6 +468,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -602,452 +661,457 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
-    <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
-    <hyperlink ref="A29" r:id="rId28"/>
-    <hyperlink ref="A30" r:id="rId29"/>
-    <hyperlink ref="A31" r:id="rId30"/>
-    <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A33" r:id="rId32"/>
-    <hyperlink ref="A34" r:id="rId33"/>
-    <hyperlink ref="A35" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
-    <hyperlink ref="A37" r:id="rId36"/>
-    <hyperlink ref="A38" r:id="rId37"/>
-    <hyperlink ref="A39" r:id="rId38"/>
-    <hyperlink ref="A40" r:id="rId39"/>
-    <hyperlink ref="A41" r:id="rId40"/>
-    <hyperlink ref="A42" r:id="rId41"/>
-    <hyperlink ref="A43" r:id="rId42"/>
-    <hyperlink ref="A44" r:id="rId43"/>
-    <hyperlink ref="A45" r:id="rId44"/>
-    <hyperlink ref="A46" r:id="rId45"/>
-    <hyperlink ref="A47" r:id="rId46"/>
-    <hyperlink ref="A48" r:id="rId47"/>
-    <hyperlink ref="A49" r:id="rId48"/>
-    <hyperlink ref="A50" r:id="rId49"/>
-    <hyperlink ref="A51" r:id="rId50"/>
-    <hyperlink ref="A52" r:id="rId51"/>
-    <hyperlink ref="A53" r:id="rId52"/>
-    <hyperlink ref="A54" r:id="rId53"/>
-    <hyperlink ref="A55" r:id="rId54"/>
-    <hyperlink ref="A56" r:id="rId55"/>
-    <hyperlink ref="A57" r:id="rId56"/>
-    <hyperlink ref="A58" r:id="rId57"/>
-    <hyperlink ref="A59" r:id="rId58"/>
-    <hyperlink ref="A60" r:id="rId59"/>
-    <hyperlink ref="A61" r:id="rId60"/>
-    <hyperlink ref="A62" r:id="rId61"/>
-    <hyperlink ref="A63" r:id="rId62"/>
-    <hyperlink ref="A64" r:id="rId63"/>
-    <hyperlink ref="A65" r:id="rId64"/>
-    <hyperlink ref="A66" r:id="rId65"/>
-    <hyperlink ref="A67" r:id="rId66"/>
-    <hyperlink ref="A68" r:id="rId67"/>
-    <hyperlink ref="A69" r:id="rId68"/>
-    <hyperlink ref="A70" r:id="rId69"/>
-    <hyperlink ref="A71" r:id="rId70"/>
-    <hyperlink ref="A72" r:id="rId71"/>
-    <hyperlink ref="A73" r:id="rId72"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A37" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A38" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A39" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A40" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A41" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A51" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A52" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A53" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A54" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A56" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A58" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A59" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A72" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A73" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A4" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>